<commit_message>
updated titles and author
</commit_message>
<xml_diff>
--- a/assets/resources/documents/FedRAMP_Low_Security_Controls.xlsx
+++ b/assets/resources/documents/FedRAMP_Low_Security_Controls.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sara.herbst/Box/TC Visual Design/Client/GSA/FedRAMP/Web/1.0 FedRAMP.gov/FedRAMP Documents &amp; Templates/documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4AB44C-1CCD-FF43-AD6B-16F156E66272}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="27340" windowHeight="15680"/>
+    <workbookView xWindow="300" yWindow="460" windowWidth="27340" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Security Controls Preface" sheetId="3" r:id="rId1"/>
@@ -13,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'HHH Low Baseline Controls'!$A$2:$J$128</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2806,7 +2812,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3529,22 +3535,25 @@
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 3 2" xfId="5"/>
-    <cellStyle name="Normal 4" xfId="6"/>
-    <cellStyle name="Normal 4 2" xfId="7"/>
-    <cellStyle name="Normal 4 2 2" xfId="8"/>
-    <cellStyle name="Normal 4 2 3" xfId="9"/>
-    <cellStyle name="Normal 5" xfId="3"/>
-    <cellStyle name="Normal 6" xfId="10"/>
-    <cellStyle name="Normal 7" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 4 2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 4 2 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 6" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 7" xfId="1" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3567,7 +3576,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3882,14 +3897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -3902,14 +3917,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M383"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="73" customWidth="1"/>
     <col min="2" max="2" width="6" style="60" customWidth="1"/>
@@ -3923,7 +3938,7 @@
     <col min="10" max="10" width="9.140625" style="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="61" customFormat="1" ht="16" thickBot="1">
+    <row r="1" spans="1:13" s="61" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="70"/>
       <c r="B1" s="17"/>
       <c r="C1" s="12" t="s">
@@ -3942,7 +3957,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="37" thickBot="1">
+    <row r="2" spans="1:13" ht="43" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
         <v>594</v>
       </c>
@@ -3977,7 +3992,7 @@
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="220">
+    <row r="3" spans="1:13" ht="260" x14ac:dyDescent="0.2">
       <c r="A3" s="72">
         <v>1</v>
       </c>
@@ -4012,7 +4027,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" ht="409">
+    <row r="4" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="72">
         <v>2</v>
       </c>
@@ -4047,7 +4062,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" ht="143">
+    <row r="5" spans="1:13" ht="169" x14ac:dyDescent="0.2">
       <c r="A5" s="72">
         <v>3</v>
       </c>
@@ -4076,7 +4091,7 @@
       <c r="L5" s="2"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" ht="165">
+    <row r="6" spans="1:13" ht="195" x14ac:dyDescent="0.2">
       <c r="A6" s="72">
         <v>4</v>
       </c>
@@ -4109,7 +4124,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="298.25" customHeight="1">
+    <row r="7" spans="1:13" ht="298.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="72">
         <v>5</v>
       </c>
@@ -4144,7 +4159,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:13" ht="242">
+    <row r="8" spans="1:13" ht="308" x14ac:dyDescent="0.2">
       <c r="A8" s="72">
         <v>6</v>
       </c>
@@ -4173,7 +4188,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" ht="220">
+    <row r="9" spans="1:13" ht="260" x14ac:dyDescent="0.2">
       <c r="A9" s="72">
         <v>7</v>
       </c>
@@ -4202,7 +4217,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" ht="110">
+    <row r="10" spans="1:13" ht="130" x14ac:dyDescent="0.2">
       <c r="A10" s="72">
         <v>8</v>
       </c>
@@ -4231,7 +4246,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" ht="275">
+    <row r="11" spans="1:13" ht="332" x14ac:dyDescent="0.2">
       <c r="A11" s="72">
         <v>9</v>
       </c>
@@ -4260,7 +4275,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" ht="407">
+    <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" s="72">
         <v>10</v>
       </c>
@@ -4289,7 +4304,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" ht="221.5" customHeight="1">
+    <row r="13" spans="1:13" ht="221.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="72">
         <v>11</v>
       </c>
@@ -4322,7 +4337,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" ht="242">
+    <row r="14" spans="1:13" ht="284" x14ac:dyDescent="0.2">
       <c r="A14" s="72">
         <v>12</v>
       </c>
@@ -4357,7 +4372,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="1:13" ht="154">
+    <row r="15" spans="1:13" ht="195" x14ac:dyDescent="0.2">
       <c r="A15" s="72">
         <v>13</v>
       </c>
@@ -4392,7 +4407,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="1:13" ht="249.5" customHeight="1">
+    <row r="16" spans="1:13" ht="249.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="72">
         <v>14</v>
       </c>
@@ -4427,7 +4442,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="1:13" ht="132">
+    <row r="17" spans="1:13" ht="156" x14ac:dyDescent="0.2">
       <c r="A17" s="72">
         <v>15</v>
       </c>
@@ -4462,7 +4477,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13" ht="231">
+    <row r="18" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A18" s="72">
         <v>16</v>
       </c>
@@ -4497,7 +4512,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="359.5" customHeight="1">
+    <row r="19" spans="1:13" ht="359.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="72">
         <v>17</v>
       </c>
@@ -4532,7 +4547,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" ht="110">
+    <row r="20" spans="1:13" ht="143" x14ac:dyDescent="0.2">
       <c r="A20" s="72">
         <v>18</v>
       </c>
@@ -4561,7 +4576,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" ht="99">
+    <row r="21" spans="1:13" ht="117" x14ac:dyDescent="0.2">
       <c r="A21" s="72">
         <v>19</v>
       </c>
@@ -4590,7 +4605,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13" ht="143">
+    <row r="22" spans="1:13" ht="169" x14ac:dyDescent="0.2">
       <c r="A22" s="72">
         <v>20</v>
       </c>
@@ -4625,7 +4640,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" ht="176">
+    <row r="23" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A23" s="72">
         <v>21</v>
       </c>
@@ -4660,7 +4675,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13" ht="154">
+    <row r="24" spans="1:13" ht="182" x14ac:dyDescent="0.2">
       <c r="A24" s="72">
         <v>22</v>
       </c>
@@ -4689,7 +4704,7 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="1:13" ht="88">
+    <row r="25" spans="1:13" ht="117" x14ac:dyDescent="0.2">
       <c r="A25" s="72">
         <v>23</v>
       </c>
@@ -4718,7 +4733,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" ht="121">
+    <row r="26" spans="1:13" ht="143" x14ac:dyDescent="0.2">
       <c r="A26" s="72">
         <v>24</v>
       </c>
@@ -4753,7 +4768,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" ht="143">
+    <row r="27" spans="1:13" ht="169" x14ac:dyDescent="0.2">
       <c r="A27" s="72">
         <v>25</v>
       </c>
@@ -4788,7 +4803,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" ht="242">
+    <row r="28" spans="1:13" ht="284" x14ac:dyDescent="0.2">
       <c r="A28" s="72">
         <v>26</v>
       </c>
@@ -4823,7 +4838,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="1:13" ht="407">
+    <row r="29" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A29" s="72">
         <v>27</v>
       </c>
@@ -4858,7 +4873,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="1:13" ht="306.5" customHeight="1">
+    <row r="30" spans="1:13" ht="306.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="72">
         <v>28</v>
       </c>
@@ -4889,7 +4904,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="1:13" ht="231">
+    <row r="31" spans="1:13" ht="296" x14ac:dyDescent="0.2">
       <c r="A31" s="72">
         <v>29</v>
       </c>
@@ -4924,7 +4939,7 @@
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
     </row>
-    <row r="32" spans="1:13" ht="132">
+    <row r="32" spans="1:13" ht="156" x14ac:dyDescent="0.2">
       <c r="A32" s="72">
         <v>30</v>
       </c>
@@ -4959,7 +4974,7 @@
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
     </row>
-    <row r="33" spans="1:13" ht="275">
+    <row r="33" spans="1:13" ht="332" x14ac:dyDescent="0.2">
       <c r="A33" s="72">
         <v>31</v>
       </c>
@@ -4994,7 +5009,7 @@
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
     </row>
-    <row r="34" spans="1:13" ht="345" customHeight="1">
+    <row r="34" spans="1:13" ht="345" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="72">
         <v>32</v>
       </c>
@@ -5029,7 +5044,7 @@
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
     </row>
-    <row r="35" spans="1:13" ht="154">
+    <row r="35" spans="1:13" ht="182" x14ac:dyDescent="0.2">
       <c r="A35" s="72">
         <v>33</v>
       </c>
@@ -5058,7 +5073,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13" ht="231">
+    <row r="36" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A36" s="72">
         <v>34</v>
       </c>
@@ -5093,7 +5108,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" ht="143">
+    <row r="37" spans="1:13" ht="182" x14ac:dyDescent="0.2">
       <c r="A37" s="72">
         <v>35</v>
       </c>
@@ -5122,7 +5137,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13" ht="175.25" customHeight="1">
+    <row r="38" spans="1:13" ht="175.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="72">
         <v>36</v>
       </c>
@@ -5151,7 +5166,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" ht="352">
+    <row r="39" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A39" s="72">
         <v>37</v>
       </c>
@@ -5186,7 +5201,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13" ht="209">
+    <row r="40" spans="1:13" ht="247" x14ac:dyDescent="0.2">
       <c r="A40" s="72">
         <v>38</v>
       </c>
@@ -5221,7 +5236,7 @@
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
     </row>
-    <row r="41" spans="1:13" ht="187">
+    <row r="41" spans="1:13" ht="247" x14ac:dyDescent="0.2">
       <c r="A41" s="72">
         <v>39</v>
       </c>
@@ -5256,7 +5271,7 @@
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
     </row>
-    <row r="42" spans="1:13" ht="153.5" customHeight="1">
+    <row r="42" spans="1:13" ht="153.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="72">
         <v>40</v>
       </c>
@@ -5285,7 +5300,7 @@
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
     </row>
-    <row r="43" spans="1:13" ht="165">
+    <row r="43" spans="1:13" ht="208" x14ac:dyDescent="0.2">
       <c r="A43" s="72">
         <v>41</v>
       </c>
@@ -5318,7 +5333,7 @@
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
     </row>
-    <row r="44" spans="1:13" ht="231">
+    <row r="44" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A44" s="72">
         <v>42</v>
       </c>
@@ -5351,7 +5366,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:13" ht="374">
+    <row r="45" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" s="72">
         <v>43</v>
       </c>
@@ -5386,7 +5401,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:13" ht="176">
+    <row r="46" spans="1:13" ht="208" x14ac:dyDescent="0.2">
       <c r="A46" s="72">
         <v>44</v>
       </c>
@@ -5419,7 +5434,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13" ht="174" customHeight="1">
+    <row r="47" spans="1:13" ht="174" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="72">
         <v>45</v>
       </c>
@@ -5454,7 +5469,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13" ht="200" customHeight="1">
+    <row r="48" spans="1:13" ht="200" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="72">
         <v>46</v>
       </c>
@@ -5489,7 +5504,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
     </row>
-    <row r="49" spans="1:13" ht="143">
+    <row r="49" spans="1:13" ht="195" x14ac:dyDescent="0.2">
       <c r="A49" s="72">
         <v>47</v>
       </c>
@@ -5518,7 +5533,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
     </row>
-    <row r="50" spans="1:13" ht="242">
+    <row r="50" spans="1:13" ht="284" x14ac:dyDescent="0.2">
       <c r="A50" s="72">
         <v>48</v>
       </c>
@@ -5553,7 +5568,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13" ht="341">
+    <row r="51" spans="1:13" ht="392" x14ac:dyDescent="0.2">
       <c r="A51" s="72">
         <v>49</v>
       </c>
@@ -5582,7 +5597,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13" ht="44">
+    <row r="52" spans="1:13" ht="56" x14ac:dyDescent="0.2">
       <c r="A52" s="72">
         <v>50</v>
       </c>
@@ -5611,7 +5626,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13" ht="108.5" customHeight="1">
+    <row r="53" spans="1:13" ht="108.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="72">
         <v>51</v>
       </c>
@@ -5642,7 +5657,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
     </row>
-    <row r="54" spans="1:13" ht="225.5" customHeight="1">
+    <row r="54" spans="1:13" ht="225.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="72">
         <v>52</v>
       </c>
@@ -5677,7 +5692,7 @@
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
     </row>
-    <row r="55" spans="1:13" ht="341">
+    <row r="55" spans="1:13" ht="392" x14ac:dyDescent="0.2">
       <c r="A55" s="72">
         <v>53</v>
       </c>
@@ -5710,7 +5725,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13" ht="187">
+    <row r="56" spans="1:13" ht="234" x14ac:dyDescent="0.2">
       <c r="A56" s="72">
         <v>54</v>
       </c>
@@ -5745,7 +5760,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13" ht="66">
+    <row r="57" spans="1:13" ht="78" x14ac:dyDescent="0.2">
       <c r="A57" s="72">
         <v>55</v>
       </c>
@@ -5774,7 +5789,7 @@
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
-    <row r="58" spans="1:13" ht="165">
+    <row r="58" spans="1:13" ht="195" x14ac:dyDescent="0.2">
       <c r="A58" s="72">
         <v>56</v>
       </c>
@@ -5803,7 +5818,7 @@
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
     </row>
-    <row r="59" spans="1:13" ht="137.5" customHeight="1">
+    <row r="59" spans="1:13" ht="137.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="72">
         <v>57</v>
       </c>
@@ -5832,7 +5847,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13" ht="192.5" customHeight="1">
+    <row r="60" spans="1:13" ht="192.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="72">
         <v>58</v>
       </c>
@@ -5861,7 +5876,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13" ht="106.75" customHeight="1">
+    <row r="61" spans="1:13" ht="106.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="72">
         <v>59</v>
       </c>
@@ -5890,7 +5905,7 @@
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
     </row>
-    <row r="62" spans="1:13" ht="88">
+    <row r="62" spans="1:13" ht="104" x14ac:dyDescent="0.2">
       <c r="A62" s="72">
         <v>60</v>
       </c>
@@ -5919,7 +5934,7 @@
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
     </row>
-    <row r="63" spans="1:13" ht="77">
+    <row r="63" spans="1:13" ht="91" x14ac:dyDescent="0.2">
       <c r="A63" s="72">
         <v>61</v>
       </c>
@@ -5948,7 +5963,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13" ht="88">
+    <row r="64" spans="1:13" ht="104" x14ac:dyDescent="0.2">
       <c r="A64" s="72">
         <v>62</v>
       </c>
@@ -5977,7 +5992,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" ht="252" customHeight="1">
+    <row r="65" spans="1:13" ht="252" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="72">
         <v>63</v>
       </c>
@@ -6012,7 +6027,7 @@
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
     </row>
-    <row r="66" spans="1:13" ht="177.5" customHeight="1">
+    <row r="66" spans="1:13" ht="177.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="72">
         <v>64</v>
       </c>
@@ -6045,7 +6060,7 @@
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
     </row>
-    <row r="67" spans="1:13" ht="198">
+    <row r="67" spans="1:13" ht="234" x14ac:dyDescent="0.2">
       <c r="A67" s="72">
         <v>65</v>
       </c>
@@ -6076,7 +6091,7 @@
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
     </row>
-    <row r="68" spans="1:13" ht="99">
+    <row r="68" spans="1:13" ht="117" x14ac:dyDescent="0.2">
       <c r="A68" s="72">
         <v>66</v>
       </c>
@@ -6105,7 +6120,7 @@
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
     </row>
-    <row r="69" spans="1:13" ht="165">
+    <row r="69" spans="1:13" ht="195" x14ac:dyDescent="0.2">
       <c r="A69" s="72">
         <v>67</v>
       </c>
@@ -6140,7 +6155,7 @@
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
     </row>
-    <row r="70" spans="1:13" ht="66">
+    <row r="70" spans="1:13" ht="78" x14ac:dyDescent="0.2">
       <c r="A70" s="72">
         <v>68</v>
       </c>
@@ -6169,7 +6184,7 @@
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
     </row>
-    <row r="71" spans="1:13" ht="319">
+    <row r="71" spans="1:13" ht="368" x14ac:dyDescent="0.2">
       <c r="A71" s="72">
         <v>69</v>
       </c>
@@ -6204,7 +6219,7 @@
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
     </row>
-    <row r="72" spans="1:13" ht="231">
+    <row r="72" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A72" s="72">
         <v>70</v>
       </c>
@@ -6239,7 +6254,7 @@
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
     </row>
-    <row r="73" spans="1:13" ht="253">
+    <row r="73" spans="1:13" ht="320" x14ac:dyDescent="0.2">
       <c r="A73" s="72">
         <v>71</v>
       </c>
@@ -6268,7 +6283,7 @@
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
     </row>
-    <row r="74" spans="1:13" ht="209">
+    <row r="74" spans="1:13" ht="247" x14ac:dyDescent="0.2">
       <c r="A74" s="72">
         <v>72</v>
       </c>
@@ -6297,7 +6312,7 @@
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
     </row>
-    <row r="75" spans="1:13" ht="217.75" customHeight="1">
+    <row r="75" spans="1:13" ht="217.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="72">
         <v>73</v>
       </c>
@@ -6326,7 +6341,7 @@
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
     </row>
-    <row r="76" spans="1:13" ht="231">
+    <row r="76" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A76" s="72">
         <v>74</v>
       </c>
@@ -6359,7 +6374,7 @@
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
     </row>
-    <row r="77" spans="1:13" ht="110">
+    <row r="77" spans="1:13" ht="130" x14ac:dyDescent="0.2">
       <c r="A77" s="72">
         <v>75</v>
       </c>
@@ -6388,7 +6403,7 @@
       <c r="L77" s="8"/>
       <c r="M77" s="8"/>
     </row>
-    <row r="78" spans="1:13" ht="274.75" customHeight="1">
+    <row r="78" spans="1:13" ht="274.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="72">
         <v>76</v>
       </c>
@@ -6417,7 +6432,7 @@
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
     </row>
-    <row r="79" spans="1:13" ht="187">
+    <row r="79" spans="1:13" ht="234" x14ac:dyDescent="0.2">
       <c r="A79" s="72">
         <v>77</v>
       </c>
@@ -6446,7 +6461,7 @@
       <c r="L79" s="4"/>
       <c r="M79" s="4"/>
     </row>
-    <row r="80" spans="1:13" ht="242">
+    <row r="80" spans="1:13" ht="284" x14ac:dyDescent="0.2">
       <c r="A80" s="72">
         <v>78</v>
       </c>
@@ -6481,7 +6496,7 @@
       <c r="L80" s="4"/>
       <c r="M80" s="4"/>
     </row>
-    <row r="81" spans="1:13" ht="154">
+    <row r="81" spans="1:13" ht="182" x14ac:dyDescent="0.2">
       <c r="A81" s="72">
         <v>79</v>
       </c>
@@ -6514,7 +6529,7 @@
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
     </row>
-    <row r="82" spans="1:13" ht="319">
+    <row r="82" spans="1:13" ht="392" x14ac:dyDescent="0.2">
       <c r="A82" s="72">
         <v>80</v>
       </c>
@@ -6547,7 +6562,7 @@
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
     </row>
-    <row r="83" spans="1:13" ht="143">
+    <row r="83" spans="1:13" ht="169" x14ac:dyDescent="0.2">
       <c r="A83" s="72">
         <v>81</v>
       </c>
@@ -6580,7 +6595,7 @@
       <c r="L83" s="4"/>
       <c r="M83" s="4"/>
     </row>
-    <row r="84" spans="1:13" ht="110">
+    <row r="84" spans="1:13" ht="130" x14ac:dyDescent="0.2">
       <c r="A84" s="72">
         <v>82</v>
       </c>
@@ -6613,7 +6628,7 @@
       <c r="L84" s="4"/>
       <c r="M84" s="4"/>
     </row>
-    <row r="85" spans="1:13" ht="88">
+    <row r="85" spans="1:13" ht="104" x14ac:dyDescent="0.2">
       <c r="A85" s="72">
         <v>83</v>
       </c>
@@ -6642,7 +6657,7 @@
       <c r="L85" s="4"/>
       <c r="M85" s="4"/>
     </row>
-    <row r="86" spans="1:13" ht="99">
+    <row r="86" spans="1:13" ht="117" x14ac:dyDescent="0.2">
       <c r="A86" s="72">
         <v>84</v>
       </c>
@@ -6671,7 +6686,7 @@
       <c r="L86" s="4"/>
       <c r="M86" s="4"/>
     </row>
-    <row r="87" spans="1:13" ht="110">
+    <row r="87" spans="1:13" ht="130" x14ac:dyDescent="0.2">
       <c r="A87" s="72">
         <v>85</v>
       </c>
@@ -6706,7 +6721,7 @@
       <c r="L87" s="4"/>
       <c r="M87" s="4"/>
     </row>
-    <row r="88" spans="1:13" ht="99">
+    <row r="88" spans="1:13" ht="117" x14ac:dyDescent="0.2">
       <c r="A88" s="72">
         <v>86</v>
       </c>
@@ -6735,7 +6750,7 @@
       <c r="L88" s="4"/>
       <c r="M88" s="4"/>
     </row>
-    <row r="89" spans="1:13" ht="88">
+    <row r="89" spans="1:13" ht="117" x14ac:dyDescent="0.2">
       <c r="A89" s="72">
         <v>87</v>
       </c>
@@ -6768,7 +6783,7 @@
       <c r="L89" s="4"/>
       <c r="M89" s="4"/>
     </row>
-    <row r="90" spans="1:13" ht="231">
+    <row r="90" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A90" s="72">
         <v>88</v>
       </c>
@@ -6801,7 +6816,7 @@
       <c r="L90" s="4"/>
       <c r="M90" s="4"/>
     </row>
-    <row r="91" spans="1:13" ht="409">
+    <row r="91" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A91" s="72">
         <v>89</v>
       </c>
@@ -6834,7 +6849,7 @@
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
     </row>
-    <row r="92" spans="1:13" ht="220">
+    <row r="92" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A92" s="72">
         <v>90</v>
       </c>
@@ -6867,7 +6882,7 @@
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
     </row>
-    <row r="93" spans="1:13" ht="231">
+    <row r="93" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A93" s="72">
         <v>91</v>
       </c>
@@ -6902,7 +6917,7 @@
       <c r="L93" s="4"/>
       <c r="M93" s="4"/>
     </row>
-    <row r="94" spans="1:13" ht="143">
+    <row r="94" spans="1:13" ht="169" x14ac:dyDescent="0.2">
       <c r="A94" s="72">
         <v>92</v>
       </c>
@@ -6935,7 +6950,7 @@
       <c r="L94" s="4"/>
       <c r="M94" s="4"/>
     </row>
-    <row r="95" spans="1:13" ht="156">
+    <row r="95" spans="1:13" ht="182" x14ac:dyDescent="0.2">
       <c r="A95" s="72">
         <v>93</v>
       </c>
@@ -6968,7 +6983,7 @@
       <c r="L95" s="4"/>
       <c r="M95" s="4"/>
     </row>
-    <row r="96" spans="1:13" ht="277.75" customHeight="1">
+    <row r="96" spans="1:13" ht="277.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="72">
         <v>94</v>
       </c>
@@ -7001,7 +7016,7 @@
       <c r="L96" s="4"/>
       <c r="M96" s="4"/>
     </row>
-    <row r="97" spans="1:13" ht="209">
+    <row r="97" spans="1:13" ht="247" x14ac:dyDescent="0.2">
       <c r="A97" s="72">
         <v>95</v>
       </c>
@@ -7036,7 +7051,7 @@
       <c r="L97" s="4"/>
       <c r="M97" s="4"/>
     </row>
-    <row r="98" spans="1:13" ht="165">
+    <row r="98" spans="1:13" ht="208" x14ac:dyDescent="0.2">
       <c r="A98" s="72">
         <v>96</v>
       </c>
@@ -7069,7 +7084,7 @@
       <c r="L98" s="4"/>
       <c r="M98" s="4"/>
     </row>
-    <row r="99" spans="1:13" ht="242">
+    <row r="99" spans="1:13" ht="296" x14ac:dyDescent="0.2">
       <c r="A99" s="72">
         <v>97</v>
       </c>
@@ -7102,7 +7117,7 @@
       <c r="L99" s="4"/>
       <c r="M99" s="4"/>
     </row>
-    <row r="100" spans="1:13" ht="154">
+    <row r="100" spans="1:13" ht="182" x14ac:dyDescent="0.2">
       <c r="A100" s="72">
         <v>98</v>
       </c>
@@ -7131,7 +7146,7 @@
       <c r="L100" s="8"/>
       <c r="M100" s="8"/>
     </row>
-    <row r="101" spans="1:13" ht="231">
+    <row r="101" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A101" s="72">
         <v>99</v>
       </c>
@@ -7164,7 +7179,7 @@
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
     </row>
-    <row r="102" spans="1:13" ht="209">
+    <row r="102" spans="1:13" ht="272" x14ac:dyDescent="0.2">
       <c r="A102" s="72">
         <v>100</v>
       </c>
@@ -7193,7 +7208,7 @@
       <c r="L102" s="4"/>
       <c r="M102" s="4"/>
     </row>
-    <row r="103" spans="1:13" ht="341">
+    <row r="103" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A103" s="72">
         <v>101</v>
       </c>
@@ -7228,7 +7243,7 @@
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
     </row>
-    <row r="104" spans="1:13" ht="319">
+    <row r="104" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A104" s="72">
         <v>102</v>
       </c>
@@ -7263,7 +7278,7 @@
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
     </row>
-    <row r="105" spans="1:13" ht="249" customHeight="1">
+    <row r="105" spans="1:13" ht="249" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="72">
         <v>103</v>
       </c>
@@ -7296,7 +7311,7 @@
       <c r="L105" s="4"/>
       <c r="M105" s="4"/>
     </row>
-    <row r="106" spans="1:13" ht="143">
+    <row r="106" spans="1:13" ht="169" x14ac:dyDescent="0.2">
       <c r="A106" s="72">
         <v>104</v>
       </c>
@@ -7325,7 +7340,7 @@
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
     </row>
-    <row r="107" spans="1:13" ht="286">
+    <row r="107" spans="1:13" ht="332" x14ac:dyDescent="0.2">
       <c r="A107" s="72">
         <v>105</v>
       </c>
@@ -7354,7 +7369,7 @@
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
     </row>
-    <row r="108" spans="1:13" ht="363">
+    <row r="108" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A108" s="72">
         <v>106</v>
       </c>
@@ -7385,7 +7400,7 @@
       <c r="L108" s="4"/>
       <c r="M108" s="4"/>
     </row>
-    <row r="109" spans="1:13" ht="297">
+    <row r="109" spans="1:13" ht="344" x14ac:dyDescent="0.2">
       <c r="A109" s="72">
         <v>107</v>
       </c>
@@ -7414,7 +7429,7 @@
       <c r="L109" s="8"/>
       <c r="M109" s="8"/>
     </row>
-    <row r="110" spans="1:13" ht="264">
+    <row r="110" spans="1:13" ht="320" x14ac:dyDescent="0.2">
       <c r="A110" s="72">
         <v>108</v>
       </c>
@@ -7447,7 +7462,7 @@
       <c r="L110" s="4"/>
       <c r="M110" s="4"/>
     </row>
-    <row r="111" spans="1:13" ht="253.25" customHeight="1">
+    <row r="111" spans="1:13" ht="253.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="72">
         <v>109</v>
       </c>
@@ -7480,7 +7495,7 @@
       <c r="L111" s="4"/>
       <c r="M111" s="4"/>
     </row>
-    <row r="112" spans="1:13" ht="110">
+    <row r="112" spans="1:13" ht="143" x14ac:dyDescent="0.2">
       <c r="A112" s="72">
         <v>110</v>
       </c>
@@ -7509,7 +7524,7 @@
       <c r="L112" s="4"/>
       <c r="M112" s="4"/>
     </row>
-    <row r="113" spans="1:13" ht="209">
+    <row r="113" spans="1:13" ht="260" x14ac:dyDescent="0.2">
       <c r="A113" s="72">
         <v>111</v>
       </c>
@@ -7538,7 +7553,7 @@
       <c r="L113" s="4"/>
       <c r="M113" s="4"/>
     </row>
-    <row r="114" spans="1:13" ht="121">
+    <row r="114" spans="1:13" ht="143" x14ac:dyDescent="0.2">
       <c r="A114" s="72">
         <v>112</v>
       </c>
@@ -7569,7 +7584,7 @@
       <c r="L114" s="4"/>
       <c r="M114" s="4"/>
     </row>
-    <row r="115" spans="1:13" ht="154">
+    <row r="115" spans="1:13" ht="195" x14ac:dyDescent="0.2">
       <c r="A115" s="72">
         <v>113</v>
       </c>
@@ -7602,7 +7617,7 @@
       <c r="L115" s="4"/>
       <c r="M115" s="4"/>
     </row>
-    <row r="116" spans="1:13" ht="110">
+    <row r="116" spans="1:13" ht="130" x14ac:dyDescent="0.2">
       <c r="A116" s="72">
         <v>114</v>
       </c>
@@ -7637,7 +7652,7 @@
       <c r="L116" s="4"/>
       <c r="M116" s="4"/>
     </row>
-    <row r="117" spans="1:13" ht="187">
+    <row r="117" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A117" s="72">
         <v>115</v>
       </c>
@@ -7666,7 +7681,7 @@
       <c r="L117" s="4"/>
       <c r="M117" s="4"/>
     </row>
-    <row r="118" spans="1:13" ht="132">
+    <row r="118" spans="1:13" ht="156" x14ac:dyDescent="0.2">
       <c r="A118" s="72">
         <v>116</v>
       </c>
@@ -7695,7 +7710,7 @@
       <c r="L118" s="4"/>
       <c r="M118" s="4"/>
     </row>
-    <row r="119" spans="1:13" ht="165">
+    <row r="119" spans="1:13" ht="208" x14ac:dyDescent="0.2">
       <c r="A119" s="72">
         <v>117</v>
       </c>
@@ -7724,7 +7739,7 @@
       <c r="L119" s="4"/>
       <c r="M119" s="4"/>
     </row>
-    <row r="120" spans="1:13" ht="110">
+    <row r="120" spans="1:13" ht="143" x14ac:dyDescent="0.2">
       <c r="A120" s="72">
         <v>118</v>
       </c>
@@ -7753,7 +7768,7 @@
       <c r="L120" s="4"/>
       <c r="M120" s="4"/>
     </row>
-    <row r="121" spans="1:13" ht="242">
+    <row r="121" spans="1:13" ht="284" x14ac:dyDescent="0.2">
       <c r="A121" s="72">
         <v>119</v>
       </c>
@@ -7786,7 +7801,7 @@
       <c r="L121" s="4"/>
       <c r="M121" s="4"/>
     </row>
-    <row r="122" spans="1:13" ht="280.25" customHeight="1">
+    <row r="122" spans="1:13" ht="280.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="72">
         <v>120</v>
       </c>
@@ -7819,7 +7834,7 @@
       <c r="L122" s="4"/>
       <c r="M122" s="4"/>
     </row>
-    <row r="123" spans="1:13" ht="352">
+    <row r="123" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A123" s="72">
         <v>121</v>
       </c>
@@ -7852,7 +7867,7 @@
       <c r="L123" s="4"/>
       <c r="M123" s="4"/>
     </row>
-    <row r="124" spans="1:13" ht="374">
+    <row r="124" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A124" s="72">
         <v>122</v>
       </c>
@@ -7883,7 +7898,7 @@
       <c r="L124" s="4"/>
       <c r="M124" s="4"/>
     </row>
-    <row r="125" spans="1:13" ht="198">
+    <row r="125" spans="1:13" ht="247" x14ac:dyDescent="0.2">
       <c r="A125" s="72">
         <v>123</v>
       </c>
@@ -7916,7 +7931,7 @@
       <c r="L125" s="4"/>
       <c r="M125" s="4"/>
     </row>
-    <row r="126" spans="1:13" ht="121">
+    <row r="126" spans="1:13" ht="143" x14ac:dyDescent="0.2">
       <c r="A126" s="72">
         <v>124</v>
       </c>
@@ -7945,7 +7960,7 @@
       <c r="L126" s="7"/>
       <c r="M126" s="7"/>
     </row>
-    <row r="127" spans="1:13" ht="121">
+    <row r="127" spans="1:13" ht="156" x14ac:dyDescent="0.2">
       <c r="A127" s="72">
         <v>125</v>
       </c>
@@ -7974,7 +7989,7 @@
       <c r="L127" s="7"/>
       <c r="M127" s="7"/>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B128" s="49"/>
       <c r="C128" s="49" t="s">
         <v>15</v>
@@ -7992,7 +8007,7 @@
       <c r="L128" s="10"/>
       <c r="M128" s="10"/>
     </row>
-    <row r="129" spans="2:13">
+    <row r="129" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B129" s="53"/>
       <c r="C129" s="53"/>
       <c r="D129" s="54"/>
@@ -8006,7 +8021,7 @@
       <c r="L129" s="3"/>
       <c r="M129" s="3"/>
     </row>
-    <row r="130" spans="2:13">
+    <row r="130" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B130" s="53"/>
       <c r="C130" s="53"/>
       <c r="D130" s="54"/>
@@ -8020,7 +8035,7 @@
       <c r="L130" s="3"/>
       <c r="M130" s="3"/>
     </row>
-    <row r="131" spans="2:13">
+    <row r="131" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B131" s="53"/>
       <c r="C131" s="53"/>
       <c r="D131" s="58"/>
@@ -8034,7 +8049,7 @@
       <c r="L131" s="5"/>
       <c r="M131" s="5"/>
     </row>
-    <row r="132" spans="2:13">
+    <row r="132" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B132" s="53"/>
       <c r="C132" s="53"/>
       <c r="D132" s="58"/>
@@ -8048,7 +8063,7 @@
       <c r="L132" s="3"/>
       <c r="M132" s="3"/>
     </row>
-    <row r="133" spans="2:13">
+    <row r="133" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B133" s="57"/>
       <c r="C133" s="57"/>
       <c r="D133" s="57"/>
@@ -8062,7 +8077,7 @@
       <c r="L133" s="3"/>
       <c r="M133" s="3"/>
     </row>
-    <row r="134" spans="2:13">
+    <row r="134" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B134" s="57"/>
       <c r="C134" s="57"/>
       <c r="D134" s="57"/>
@@ -8076,7 +8091,7 @@
       <c r="L134" s="3"/>
       <c r="M134" s="3"/>
     </row>
-    <row r="135" spans="2:13">
+    <row r="135" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B135" s="57"/>
       <c r="C135" s="57"/>
       <c r="D135" s="57"/>
@@ -8090,684 +8105,684 @@
       <c r="L135" s="3"/>
       <c r="M135" s="3"/>
     </row>
-    <row r="136" spans="2:13">
+    <row r="136" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F136" s="69"/>
     </row>
-    <row r="137" spans="2:13">
+    <row r="137" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F137" s="69"/>
     </row>
-    <row r="138" spans="2:13">
+    <row r="138" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F138" s="69"/>
     </row>
-    <row r="139" spans="2:13">
+    <row r="139" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F139" s="69"/>
     </row>
-    <row r="140" spans="2:13">
+    <row r="140" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F140" s="69"/>
     </row>
-    <row r="141" spans="2:13">
+    <row r="141" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F141" s="69"/>
     </row>
-    <row r="142" spans="2:13">
+    <row r="142" spans="2:13" x14ac:dyDescent="0.2">
       <c r="F142" s="69"/>
     </row>
-    <row r="253" spans="1:1">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:1">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:1">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:1">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:1">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:1">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:1">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:1">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:1">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:1">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:1">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:1">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:1">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:1">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:1">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:1">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:1">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:1">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:1">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:1">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:1">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:1">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:1">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:1">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:1">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:1">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:1">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:1">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:1">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:1">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:1">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:1">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:1">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:1">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:1">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:1">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:1">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:1">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:1">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:1">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:1">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:1">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:1">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:1">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:1">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:1">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:1">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:1">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:1">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:1">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A302" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:1">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A303" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:1">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A304" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:1">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A305" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:1">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A306" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:1">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A307" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:1">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A308" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:1">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A309" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:1">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A310" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:1">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A311" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:1">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A312" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:1">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A313" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:1">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A314" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:1">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A315" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:1">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A316" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:1">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A317" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:1">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A318" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:1">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A319" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:1">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A320" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:1">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A321" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:1">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A322" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:1">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:1">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A324" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:1">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A325" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:1">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A326" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:1">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A327" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:1">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A328" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:1">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A329" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:1">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A330" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:1">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A331" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:1">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A332" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:1">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A333" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:1">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A334" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:1">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A335" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:1">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A336" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:1">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:1">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A338" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:1">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A339" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:1">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A340" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:1">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A341" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:1">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A342" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:1">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A343" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:1">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A344" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:1">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A345" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:1">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A346" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:1">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A347" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:1">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A348" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:1">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A349" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:1">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A350" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:1">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A351" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:1">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A352" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:1">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A353" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:1">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A354" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:1">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A355" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:1">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A356" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:1">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A357" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:1">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A358" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:1">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A359" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:1">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A360" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:1">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A361" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:1">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A362" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:1">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:1">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A364" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:1">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A365" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:1">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A366" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:1">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A367" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:1">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A368" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:1">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A369" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:1">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A370" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:1">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A371" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:1">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A372" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:1">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A373" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:1">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A374" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:1">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A375" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:1">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A376" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:1">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A377" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:1">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A378" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:1">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A379" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:1">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A380" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:1">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A381" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:1">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A382" s="73">
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:1">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A383" s="73">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J128"/>
+  <autoFilter ref="A2:J128" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
   <extLst>

</xml_diff>